<commit_message>
catch for Vaule error added
</commit_message>
<xml_diff>
--- a/example_spreadsheets/game_collection.xlsx
+++ b/example_spreadsheets/game_collection.xlsx
@@ -28,6 +28,7 @@
     <sheet state="visible" name="Wii U" sheetId="23" r:id="rId26"/>
     <sheet state="visible" name="Playstation 4" sheetId="24" r:id="rId27"/>
     <sheet state="visible" name="Nintendo Switch" sheetId="25" r:id="rId28"/>
+    <sheet state="visible" name="Playstation 5" sheetId="26" r:id="rId29"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="429">
   <si>
     <t>Title</t>
   </si>
@@ -370,12 +371,24 @@
     <t>Strikers 1945 Plus</t>
   </si>
   <si>
+    <t>Alien Trilogy</t>
+  </si>
+  <si>
     <t>Castlevania Symphony Of The Night Limited Edition</t>
   </si>
   <si>
     <t>Chrono Cross</t>
   </si>
   <si>
+    <t>Crash Bandicoot</t>
+  </si>
+  <si>
+    <t>Crash Bandicoot 2 Cortex Strikes Back</t>
+  </si>
+  <si>
+    <t>Crash Bandicoot 3 Warped</t>
+  </si>
+  <si>
     <t>Dino Crisis</t>
   </si>
   <si>
@@ -385,6 +398,9 @@
     <t>Driver</t>
   </si>
   <si>
+    <t>Driver 2</t>
+  </si>
+  <si>
     <t>Fear Effect</t>
   </si>
   <si>
@@ -424,6 +440,12 @@
     <t>Overblood</t>
   </si>
   <si>
+    <t>Parasite Eve</t>
+  </si>
+  <si>
+    <t>Rayman</t>
+  </si>
+  <si>
     <t>Resident Evil</t>
   </si>
   <si>
@@ -433,12 +455,21 @@
     <t>Resident Evil 3 Nemesis</t>
   </si>
   <si>
+    <t>Resident Evil Survivor</t>
+  </si>
+  <si>
+    <t>Ridge Racer Type 4</t>
+  </si>
+  <si>
     <t>Rollcage</t>
   </si>
   <si>
     <t>Silent Hill</t>
   </si>
   <si>
+    <t>Spyro the Dragon</t>
+  </si>
+  <si>
     <t>Syphon Filter 2</t>
   </si>
   <si>
@@ -451,6 +482,9 @@
     <t>Tenchu Stealth Assassins</t>
   </si>
   <si>
+    <t>Tomb Raider</t>
+  </si>
+  <si>
     <t>Tomb Raider II</t>
   </si>
   <si>
@@ -463,7 +497,7 @@
     <t>Tomb Raider Chronicles</t>
   </si>
   <si>
-    <t>Tony Hawk</t>
+    <t>Tony Hawk's Skateboarding</t>
   </si>
   <si>
     <t>Tony Hawk 2</t>
@@ -493,12 +527,24 @@
     <t>1080 Snowboarding</t>
   </si>
   <si>
+    <t>Armorines Project Swarm</t>
+  </si>
+  <si>
     <t>Banjo Kazooie</t>
   </si>
   <si>
     <t>Banjo Tooie</t>
   </si>
   <si>
+    <t>Blast Corps</t>
+  </si>
+  <si>
+    <t>Bomberman 64</t>
+  </si>
+  <si>
+    <t>Castlevania Legacy of Darkness</t>
+  </si>
+  <si>
     <t>Conker's Bad Fur Day</t>
   </si>
   <si>
@@ -511,9 +557,21 @@
     <t>Doom 64</t>
   </si>
   <si>
+    <t>Duke Nukem 64</t>
+  </si>
+  <si>
+    <t>Extreme G</t>
+  </si>
+  <si>
+    <t>Fighters Destiny</t>
+  </si>
+  <si>
     <t>F Zero X</t>
   </si>
   <si>
+    <t>Forsaken</t>
+  </si>
+  <si>
     <t>Hybrid Heaven</t>
   </si>
   <si>
@@ -529,12 +587,27 @@
     <t>Mario Kart 64</t>
   </si>
   <si>
+    <t>Mystical Ninja Starring Goemon</t>
+  </si>
+  <si>
+    <t>Operation Winback</t>
+  </si>
+  <si>
     <t>Perfect Dark</t>
   </si>
   <si>
     <t>Pilotwings 64</t>
   </si>
   <si>
+    <t>Pokemon Snap</t>
+  </si>
+  <si>
+    <t>Quake</t>
+  </si>
+  <si>
+    <t>Quake II</t>
+  </si>
+  <si>
     <t>Rayman 2 The Great Escape</t>
   </si>
   <si>
@@ -544,6 +617,9 @@
     <t>Snowboard Kids</t>
   </si>
   <si>
+    <t>South Park</t>
+  </si>
+  <si>
     <t>Space Station Silicon Valley</t>
   </si>
   <si>
@@ -562,12 +638,27 @@
     <t>Top Gear Rally</t>
   </si>
   <si>
+    <t>Turok Dinosaur Hunter</t>
+  </si>
+  <si>
+    <t>Turok Rage Wars</t>
+  </si>
+  <si>
     <t>Turok 2 Seeds Of Evil</t>
   </si>
   <si>
     <t>Wave Race 64</t>
   </si>
   <si>
+    <t>WCW vs NWO Revenge</t>
+  </si>
+  <si>
+    <t>Wipeout</t>
+  </si>
+  <si>
+    <t>WWF No Mercy</t>
+  </si>
+  <si>
     <t>Zelda Ocarina Of Time</t>
   </si>
   <si>
@@ -583,6 +674,9 @@
     <t>The House Of The Dead 2</t>
   </si>
   <si>
+    <t>Hydro Thunder</t>
+  </si>
+  <si>
     <t>Jet Set Radio</t>
   </si>
   <si>
@@ -598,18 +692,45 @@
     <t>Shenmue II</t>
   </si>
   <si>
+    <t>Virtua Tennis</t>
+  </si>
+  <si>
+    <t>Aggressive Inline</t>
+  </si>
+  <si>
+    <t>Alone In The Dark The New Nightmare</t>
+  </si>
+  <si>
+    <t>Beyond Good and Evil</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
     <t>Burnout 3 Takedown</t>
   </si>
   <si>
+    <t>Burnout Revenge</t>
+  </si>
+  <si>
     <t>Canis Canem Edit</t>
   </si>
   <si>
+    <t>Clock Tower 3</t>
+  </si>
+  <si>
     <t>Cold Fear</t>
   </si>
   <si>
+    <t>Crazy Taxi</t>
+  </si>
+  <si>
     <t>Devil May Cry</t>
   </si>
   <si>
+    <t>Devil May Cry 3</t>
+  </si>
+  <si>
     <t>Echo Night Beyond</t>
   </si>
   <si>
@@ -625,6 +746,9 @@
     <t>Final Fantasy X</t>
   </si>
   <si>
+    <t>Final Fantasy X-2</t>
+  </si>
+  <si>
     <t>Final Fantasy XII</t>
   </si>
   <si>
@@ -643,30 +767,54 @@
     <t>Grand Theft Auto Vice City</t>
   </si>
   <si>
+    <t>Hack Infection</t>
+  </si>
+  <si>
     <t>Half Life</t>
   </si>
   <si>
     <t>Haunting Ground</t>
   </si>
   <si>
+    <t>Hitman 2</t>
+  </si>
+  <si>
     <t>Ico</t>
   </si>
   <si>
     <t>Jak And Daxter The Precursor Legacy</t>
   </si>
   <si>
-    <t>Jak &amp; Daxter 2 Renegade</t>
+    <t>Jak II Renegade</t>
+  </si>
+  <si>
+    <t>Just Cause</t>
   </si>
   <si>
     <t>Killer 7</t>
   </si>
   <si>
+    <t>Kingdom Hearts</t>
+  </si>
+  <si>
+    <t>Kingdom Hearts 2</t>
+  </si>
+  <si>
     <t>Kuon</t>
   </si>
   <si>
+    <t>Lara Croft Tomb Raider Anniversary</t>
+  </si>
+  <si>
     <t>Manhunt</t>
   </si>
   <si>
+    <t>Medal of Honor Frontline</t>
+  </si>
+  <si>
+    <t>Mercenaries</t>
+  </si>
+  <si>
     <t>Metal Gear Solid 2</t>
   </si>
   <si>
@@ -679,6 +827,9 @@
     <t>Metal Gear Solid 3 Subsistence</t>
   </si>
   <si>
+    <t>Obscure</t>
+  </si>
+  <si>
     <t>Okami</t>
   </si>
   <si>
@@ -691,6 +842,12 @@
     <t>Prince Of Persia Sands Of Time</t>
   </si>
   <si>
+    <t>Prince Of Persia Warrior Within</t>
+  </si>
+  <si>
+    <t>Prince Of Persia Two Thrones</t>
+  </si>
+  <si>
     <t>Project Zero</t>
   </si>
   <si>
@@ -706,18 +863,33 @@
     <t>Ratchet &amp; Clank</t>
   </si>
   <si>
+    <t>Ratchet &amp; Clank 2 Locked &amp; Loaded</t>
+  </si>
+  <si>
+    <t>Ratchet &amp; Clank 3</t>
+  </si>
+  <si>
     <t>Resident Evil Code Veronica X</t>
   </si>
   <si>
+    <t>Resident Evil Dead Aim</t>
+  </si>
+  <si>
     <t>Resident Evil Outbreak</t>
   </si>
   <si>
+    <t>Rogue Galaxy</t>
+  </si>
+  <si>
     <t>The Simpsons Hit And Run</t>
   </si>
   <si>
     <t>Silent Hill 2</t>
   </si>
   <si>
+    <t>Silent Hill 2 Director's Cut Platinum</t>
+  </si>
+  <si>
     <t>Silent Hill 3</t>
   </si>
   <si>
@@ -730,36 +902,93 @@
     <t>Shadow Of The Colossus</t>
   </si>
   <si>
+    <t>Smuggler's Run</t>
+  </si>
+  <si>
+    <t>State Of Emergency</t>
+  </si>
+  <si>
+    <t>Stuntman</t>
+  </si>
+  <si>
     <t>SSX</t>
   </si>
   <si>
     <t>SSX Tricky</t>
   </si>
   <si>
+    <t>SSX 3</t>
+  </si>
+  <si>
     <t>The Thing</t>
   </si>
   <si>
+    <t>Time Crisis 2</t>
+  </si>
+  <si>
     <t>Time Splitters 2</t>
   </si>
   <si>
+    <t>Tomb Raider Angel Of Darkness</t>
+  </si>
+  <si>
+    <t>Tomb Raider Legend</t>
+  </si>
+  <si>
     <t>Tony Hawk 3</t>
   </si>
   <si>
     <t>Tony Hawk 4</t>
   </si>
   <si>
+    <t>Viewtiful Joe</t>
+  </si>
+  <si>
+    <t>Virtua Fighter 4</t>
+  </si>
+  <si>
+    <t>The Warriors</t>
+  </si>
+  <si>
+    <t>XG3 Extreme G Racing</t>
+  </si>
+  <si>
     <t>Yakuza</t>
   </si>
   <si>
     <t>Zone Of The Enders</t>
   </si>
   <si>
+    <t>Zone Of The Enders 2nd Runner</t>
+  </si>
+  <si>
+    <t>Call Of Cthulhu Dark Corners Of The Earth</t>
+  </si>
+  <si>
+    <t>Chronicles Of Riddick</t>
+  </si>
+  <si>
+    <t>Doom 3</t>
+  </si>
+  <si>
+    <t>Elder Scrolls III Morrowind</t>
+  </si>
+  <si>
     <t>Halo 2</t>
   </si>
   <si>
     <t>Ninja Gaiden</t>
   </si>
   <si>
+    <t>Splinter Cell</t>
+  </si>
+  <si>
+    <t>Splinter Cell Pandora Tomorrow</t>
+  </si>
+  <si>
+    <t>Star Wars Knights Of The Old Republic</t>
+  </si>
+  <si>
     <t>Eternal Darkness</t>
   </si>
   <si>
@@ -781,12 +1010,21 @@
     <t>Resident Evil 4</t>
   </si>
   <si>
-    <t>Star Wars Rogue Squadron II</t>
+    <t>Star Fox Adventures</t>
+  </si>
+  <si>
+    <t>Star Wars Bounty Hunter</t>
+  </si>
+  <si>
+    <t>Star Wars Rogue Leader</t>
   </si>
   <si>
     <t>Super Mario Sunshine</t>
   </si>
   <si>
+    <t>Wave Race Blue Storm</t>
+  </si>
+  <si>
     <t>Zelda Wind Waker Limited Edition</t>
   </si>
   <si>
@@ -928,18 +1166,24 @@
     <t>Street Fighter IV</t>
   </si>
   <si>
-    <t>Tomb Raider</t>
-  </si>
-  <si>
-    <t>Grand Theft Auto iV</t>
+    <t>Deus Ex Human Revolution</t>
+  </si>
+  <si>
+    <t>Dishonored</t>
+  </si>
+  <si>
+    <t>Grand Theft Auto IV</t>
+  </si>
+  <si>
+    <t>ico &amp; Shadow Of The Colossus Collection</t>
+  </si>
+  <si>
+    <t>Killzone 2</t>
   </si>
   <si>
     <t>The Last Of Us</t>
   </si>
   <si>
-    <t>Killzone 2</t>
-  </si>
-  <si>
     <t>Metal Gear Solid HD Collection</t>
   </si>
   <si>
@@ -955,9 +1199,15 @@
     <t>Resident Evil 6</t>
   </si>
   <si>
+    <t>Resident Evil Revelations</t>
+  </si>
+  <si>
     <t>Resistance Fall Of Man</t>
   </si>
   <si>
+    <t>Tomb Raider Trilogy</t>
+  </si>
+  <si>
     <t>Bravely Default</t>
   </si>
   <si>
@@ -967,9 +1217,6 @@
     <t>Metroid Samus Returns</t>
   </si>
   <si>
-    <t>Resident Evil Revelations</t>
-  </si>
-  <si>
     <t>Zelda A Link Between Worlds</t>
   </si>
   <si>
@@ -994,15 +1241,24 @@
     <t>Bloodborne Game Of The Year</t>
   </si>
   <si>
+    <t>Dark Souls Trilogy</t>
+  </si>
+  <si>
     <t>Death Stranding</t>
   </si>
   <si>
-    <t>Dark Souls Trilogy</t>
+    <t>Deus Ex Mankind Divided</t>
+  </si>
+  <si>
+    <t>Dishonored 2</t>
   </si>
   <si>
     <t>Final Fantasy XII The Zodiac Age</t>
   </si>
   <si>
+    <t>The Last Guardian</t>
+  </si>
+  <si>
     <t>The Last Of Us Remastered</t>
   </si>
   <si>
@@ -1012,9 +1268,24 @@
     <t>Metal Gear Solid V The Phantom Pain</t>
   </si>
   <si>
+    <t>Nier Automata Game Of The Yorha Edition</t>
+  </si>
+  <si>
+    <t>Prey</t>
+  </si>
+  <si>
     <t>The Outer Worlds</t>
   </si>
   <si>
+    <t>Resident Evil Origins Collection</t>
+  </si>
+  <si>
+    <t>Resident Evil Revelations 2</t>
+  </si>
+  <si>
+    <t>Resident Evil 3</t>
+  </si>
+  <si>
     <t>Resident Evil 7 Biohazard</t>
   </si>
   <si>
@@ -1033,7 +1304,25 @@
     <t>Xenoblade Chronicles 2</t>
   </si>
   <si>
+    <t>Xenoblade Chronicles 3</t>
+  </si>
+  <si>
     <t>Zelda Breath Of The Wild</t>
+  </si>
+  <si>
+    <t>Deathloop</t>
+  </si>
+  <si>
+    <t>Demon's Souls</t>
+  </si>
+  <si>
+    <t>Elden Ring Launch Edition</t>
+  </si>
+  <si>
+    <t>The Last Of Us Part 1</t>
+  </si>
+  <si>
+    <t>Resident Evil Village</t>
   </si>
 </sst>
 </file>
@@ -1045,15 +1334,18 @@
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -1170,6 +1462,10 @@
 </file>
 
 <file path=xl/drawings/drawing25.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing26.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1403,9 +1699,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.0"/>
+    <col customWidth="1" min="1" max="1" width="26.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1619,9 +1915,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="49.43"/>
+    <col customWidth="1" min="1" max="1" width="43.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1651,7 +1947,7 @@
         <v>112</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>24</v>
@@ -1662,7 +1958,7 @@
         <v>113</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>24</v>
@@ -1893,7 +2189,7 @@
         <v>134</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>24</v>
@@ -2036,7 +2332,7 @@
         <v>147</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>24</v>
@@ -2044,12 +2340,133 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2066,10 +2483,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="39.0"/>
-    <col customWidth="1" min="2" max="2" width="17.57"/>
+    <col customWidth="1" min="1" max="1" width="34.13"/>
+    <col customWidth="1" min="2" max="2" width="15.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2085,7 +2502,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -2096,7 +2513,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -2107,7 +2524,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -2118,7 +2535,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -2129,18 +2546,18 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -2151,29 +2568,29 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>157</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
@@ -2184,18 +2601,18 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
@@ -2206,62 +2623,62 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
@@ -2272,7 +2689,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
@@ -2283,29 +2700,29 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
@@ -2316,7 +2733,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>23</v>
@@ -2327,18 +2744,18 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>23</v>
@@ -2349,18 +2766,18 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>23</v>
@@ -2371,18 +2788,18 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>23</v>
@@ -2393,7 +2810,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>23</v>
@@ -2404,7 +2821,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>23</v>
@@ -2415,12 +2832,243 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2437,9 +3085,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.43"/>
+    <col customWidth="1" min="1" max="1" width="18.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2455,7 +3103,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>179</v>
+        <v>209</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -2477,9 +3125,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="41.43"/>
+    <col customWidth="1" min="1" max="1" width="36.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2495,7 +3143,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -2506,7 +3154,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>181</v>
+        <v>211</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -2517,7 +3165,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -2528,7 +3176,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>183</v>
+        <v>213</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -2539,7 +3187,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>184</v>
+        <v>214</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>23</v>
@@ -2550,7 +3198,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>167</v>
+        <v>215</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -2561,7 +3209,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
@@ -2572,12 +3220,34 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>186</v>
+        <v>216</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2594,9 +3264,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="35.29"/>
+    <col customWidth="1" min="1" max="1" width="30.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2612,7 +3282,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -2623,7 +3293,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -2634,7 +3304,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>189</v>
+        <v>221</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -2645,7 +3315,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>190</v>
+        <v>222</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -2656,7 +3326,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>23</v>
@@ -2667,7 +3337,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>192</v>
+        <v>224</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -2678,7 +3348,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>193</v>
+        <v>225</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
@@ -2689,7 +3359,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
@@ -2700,7 +3370,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>195</v>
+        <v>227</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
@@ -2711,7 +3381,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>196</v>
+        <v>228</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>23</v>
@@ -2722,7 +3392,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
@@ -2733,7 +3403,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>23</v>
@@ -2744,7 +3414,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>199</v>
+        <v>231</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>23</v>
@@ -2755,7 +3425,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>200</v>
+        <v>232</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>23</v>
@@ -2766,7 +3436,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>201</v>
+        <v>233</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
@@ -2777,7 +3447,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>23</v>
@@ -2788,7 +3458,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>203</v>
+        <v>235</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
@@ -2799,7 +3469,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>204</v>
+        <v>236</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
@@ -2810,7 +3480,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>205</v>
+        <v>237</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
@@ -2821,7 +3491,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>206</v>
+        <v>238</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>23</v>
@@ -2832,7 +3502,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>207</v>
+        <v>239</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
@@ -2843,7 +3513,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>208</v>
+        <v>240</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>23</v>
@@ -2854,7 +3524,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>209</v>
+        <v>241</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>23</v>
@@ -2865,7 +3535,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>210</v>
+        <v>242</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>23</v>
@@ -2876,7 +3546,7 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>211</v>
+        <v>243</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>23</v>
@@ -2887,7 +3557,7 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>212</v>
+        <v>244</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>23</v>
@@ -2898,7 +3568,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>213</v>
+        <v>245</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>23</v>
@@ -2909,7 +3579,7 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>23</v>
@@ -2920,7 +3590,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>215</v>
+        <v>247</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>23</v>
@@ -2931,7 +3601,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>216</v>
+        <v>248</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>23</v>
@@ -2942,7 +3612,7 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>217</v>
+        <v>249</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>23</v>
@@ -2953,7 +3623,7 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>218</v>
+        <v>250</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>23</v>
@@ -2964,7 +3634,7 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>219</v>
+        <v>251</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>23</v>
@@ -2975,7 +3645,7 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>220</v>
+        <v>252</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>23</v>
@@ -2986,7 +3656,7 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>221</v>
+        <v>253</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>23</v>
@@ -2997,7 +3667,7 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>222</v>
+        <v>254</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>23</v>
@@ -3008,7 +3678,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>223</v>
+        <v>255</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>23</v>
@@ -3019,7 +3689,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>224</v>
+        <v>256</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>23</v>
@@ -3030,7 +3700,7 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>225</v>
+        <v>257</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>23</v>
@@ -3041,7 +3711,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>226</v>
+        <v>258</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>23</v>
@@ -3052,7 +3722,7 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>23</v>
@@ -3063,7 +3733,7 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>23</v>
@@ -3074,7 +3744,7 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>229</v>
+        <v>261</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>23</v>
@@ -3085,7 +3755,7 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>23</v>
@@ -3096,7 +3766,7 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>231</v>
+        <v>263</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>23</v>
@@ -3107,7 +3777,7 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>23</v>
@@ -3118,7 +3788,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>233</v>
+        <v>265</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>23</v>
@@ -3129,7 +3799,7 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>234</v>
+        <v>266</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>23</v>
@@ -3140,7 +3810,7 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>23</v>
@@ -3151,7 +3821,7 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>236</v>
+        <v>268</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>23</v>
@@ -3162,7 +3832,7 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>237</v>
+        <v>269</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>23</v>
@@ -3173,12 +3843,419 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>238</v>
+        <v>270</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" ht="18.75" customHeight="1">
+      <c r="A89" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3195,7 +4272,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="41.13"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -3210,7 +4290,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>239</v>
+        <v>308</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -3221,12 +4301,89 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>240</v>
+        <v>309</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3243,9 +4400,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="42.57"/>
+    <col customWidth="1" min="1" max="1" width="37.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3261,7 +4418,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>241</v>
+        <v>317</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -3272,7 +4429,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>242</v>
+        <v>318</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -3283,7 +4440,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>243</v>
+        <v>319</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -3294,7 +4451,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>244</v>
+        <v>320</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -3305,7 +4462,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>245</v>
+        <v>321</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>23</v>
@@ -3316,7 +4473,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -3327,7 +4484,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>246</v>
+        <v>322</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
@@ -3338,7 +4495,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>247</v>
+        <v>323</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
@@ -3349,7 +4506,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>248</v>
+        <v>324</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
@@ -3360,7 +4517,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>249</v>
+        <v>325</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>23</v>
@@ -3371,12 +4528,45 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>250</v>
+        <v>326</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3393,10 +4583,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="42.29"/>
-    <col customWidth="1" min="2" max="2" width="39.71"/>
+    <col customWidth="1" min="1" max="1" width="37.0"/>
+    <col customWidth="1" min="2" max="2" width="34.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3412,7 +4602,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>251</v>
+        <v>330</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -3423,7 +4613,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>252</v>
+        <v>331</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -3434,7 +4624,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>253</v>
+        <v>332</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -3445,7 +4635,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>254</v>
+        <v>333</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -3456,7 +4646,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>255</v>
+        <v>334</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>23</v>
@@ -3478,7 +4668,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>256</v>
+        <v>335</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
@@ -3489,7 +4679,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>257</v>
+        <v>336</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
@@ -3500,7 +4690,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>258</v>
+        <v>337</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
@@ -3511,7 +4701,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>259</v>
+        <v>338</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>23</v>
@@ -3522,7 +4712,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>260</v>
+        <v>339</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>4</v>
@@ -3533,7 +4723,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>261</v>
+        <v>340</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
@@ -3555,9 +4745,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="38.86"/>
+    <col customWidth="1" min="1" max="1" width="34.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3573,7 +4763,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>262</v>
+        <v>341</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -3584,7 +4774,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>263</v>
+        <v>342</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -3606,9 +4796,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="40.57"/>
+    <col customWidth="1" min="1" max="1" width="35.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3624,7 +4814,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>264</v>
+        <v>343</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -3635,7 +4825,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>265</v>
+        <v>344</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -3646,7 +4836,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>266</v>
+        <v>345</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -3657,7 +4847,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>267</v>
+        <v>346</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -3668,7 +4858,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>268</v>
+        <v>347</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>23</v>
@@ -3679,7 +4869,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>269</v>
+        <v>348</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -3690,7 +4880,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>214</v>
+        <v>264</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
@@ -3701,7 +4891,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>247</v>
+        <v>323</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
@@ -3712,7 +4902,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>270</v>
+        <v>349</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
@@ -3723,7 +4913,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>271</v>
+        <v>350</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>23</v>
@@ -3734,7 +4924,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>272</v>
+        <v>351</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
@@ -3745,7 +4935,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>273</v>
+        <v>352</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>23</v>
@@ -3756,7 +4946,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>274</v>
+        <v>353</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>23</v>
@@ -3767,7 +4957,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>275</v>
+        <v>354</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>23</v>
@@ -3778,10 +4968,10 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>276</v>
+        <v>355</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
@@ -3803,9 +4993,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.86"/>
+    <col customWidth="1" min="1" max="1" width="17.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3909,9 +5099,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="40.0"/>
+    <col customWidth="1" min="1" max="1" width="35.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3927,7 +5117,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>277</v>
+        <v>356</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -3938,7 +5128,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>278</v>
+        <v>357</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -3949,7 +5139,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>279</v>
+        <v>358</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -3960,7 +5150,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>280</v>
+        <v>359</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -3971,7 +5161,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>281</v>
+        <v>360</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>23</v>
@@ -3982,7 +5172,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>282</v>
+        <v>361</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -3993,7 +5183,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>283</v>
+        <v>362</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
@@ -4004,7 +5194,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>284</v>
+        <v>363</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
@@ -4015,7 +5205,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>285</v>
+        <v>364</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
@@ -4026,7 +5216,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>286</v>
+        <v>365</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>23</v>
@@ -4037,7 +5227,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>287</v>
+        <v>366</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
@@ -4048,7 +5238,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>288</v>
+        <v>367</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>23</v>
@@ -4059,7 +5249,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>289</v>
+        <v>368</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>23</v>
@@ -4070,7 +5260,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>290</v>
+        <v>369</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>23</v>
@@ -4081,7 +5271,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>291</v>
+        <v>370</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
@@ -4092,7 +5282,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>292</v>
+        <v>371</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>23</v>
@@ -4103,7 +5293,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>293</v>
+        <v>372</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
@@ -4114,7 +5304,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>294</v>
+        <v>373</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
@@ -4125,7 +5315,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>295</v>
+        <v>374</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
@@ -4136,7 +5326,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>296</v>
+        <v>375</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>23</v>
@@ -4147,7 +5337,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>297</v>
+        <v>148</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
@@ -4169,9 +5359,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="39.29"/>
+    <col customWidth="1" min="1" max="1" width="34.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4187,7 +5377,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>298</v>
+        <v>376</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -4198,7 +5388,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>299</v>
+        <v>377</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -4209,7 +5399,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>300</v>
+        <v>378</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -4220,7 +5410,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>301</v>
+        <v>379</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -4231,7 +5421,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>302</v>
+        <v>380</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>23</v>
@@ -4240,9 +5430,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>303</v>
+        <v>381</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -4253,7 +5443,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>304</v>
+        <v>382</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
@@ -4264,7 +5454,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>305</v>
+        <v>383</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
@@ -4275,12 +5465,67 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>306</v>
+        <v>384</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4297,9 +5542,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.29"/>
+    <col customWidth="1" min="1" max="1" width="24.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4315,7 +5560,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>307</v>
+        <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -4326,7 +5571,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>308</v>
+        <v>391</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -4337,7 +5582,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>309</v>
+        <v>392</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -4348,7 +5593,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>310</v>
+        <v>387</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -4359,7 +5604,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>311</v>
+        <v>393</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -4370,7 +5615,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>312</v>
+        <v>394</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -4381,7 +5626,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>313</v>
+        <v>395</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -4403,9 +5648,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="29.71"/>
+    <col customWidth="1" min="1" max="1" width="26.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4421,7 +5666,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>314</v>
+        <v>396</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -4432,7 +5677,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>315</v>
+        <v>397</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -4443,7 +5688,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>316</v>
+        <v>398</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -4465,10 +5710,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="45.0"/>
-    <col customWidth="1" min="2" max="2" width="7.57"/>
+    <col customWidth="1" min="1" max="1" width="39.38"/>
+    <col customWidth="1" min="2" max="2" width="6.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4484,7 +5729,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>317</v>
+        <v>399</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -4495,7 +5740,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>318</v>
+        <v>400</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -4506,10 +5751,10 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>319</v>
+        <v>401</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>24</v>
@@ -4517,10 +5762,10 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>320</v>
+        <v>402</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>24</v>
@@ -4528,7 +5773,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>321</v>
+        <v>403</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>23</v>
@@ -4539,7 +5784,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>322</v>
+        <v>404</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -4550,7 +5795,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>323</v>
+        <v>405</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
@@ -4561,7 +5806,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>324</v>
+        <v>406</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
@@ -4572,7 +5817,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>325</v>
+        <v>407</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
@@ -4583,7 +5828,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>130</v>
+        <v>408</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>23</v>
@@ -4594,12 +5839,111 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>326</v>
+        <v>409</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4616,9 +5960,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="39.71"/>
+    <col customWidth="1" min="1" max="1" width="34.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4634,7 +5978,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>327</v>
+        <v>417</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -4645,7 +5989,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>328</v>
+        <v>418</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -4656,7 +6000,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>329</v>
+        <v>419</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -4667,7 +6011,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>330</v>
+        <v>420</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -4678,7 +6022,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>331</v>
+        <v>421</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -4689,12 +6033,108 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>332</v>
+        <v>422</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="34.75"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4711,9 +6151,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="46.86"/>
+    <col customWidth="1" min="1" max="1" width="41.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5026,9 +6466,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.57"/>
+    <col customWidth="1" min="1" max="1" width="25.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5077,9 +6517,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="73.0"/>
+    <col customWidth="1" min="1" max="1" width="63.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5469,9 +6909,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.0"/>
+    <col customWidth="1" min="1" max="1" width="24.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5509,9 +6949,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="35.29"/>
+    <col customWidth="1" min="1" max="1" width="30.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5670,9 +7110,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="35.57"/>
+    <col customWidth="1" min="1" max="1" width="31.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5721,9 +7161,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.14"/>
+    <col customWidth="1" min="1" max="1" width="15.88"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>